<commit_message>
Added results for partial model
</commit_message>
<xml_diff>
--- a/partial/sliding_window_results_window_1.xlsx
+++ b/partial/sliding_window_results_window_1.xlsx
@@ -468,13 +468,13 @@
         <v>28.98</v>
       </c>
       <c r="C2" t="n">
-        <v>28.61942153242016</v>
+        <v>29.30314445495605</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.3605784675798382</v>
+        <v>0.3231444549560507</v>
       </c>
       <c r="E2" t="n">
-        <v>0.1300168312822245</v>
+        <v>0.1044223387688431</v>
       </c>
     </row>
     <row r="3">
@@ -482,16 +482,16 @@
         <v>48</v>
       </c>
       <c r="B3" t="n">
-        <v>29.15</v>
+        <v>29.15000000000001</v>
       </c>
       <c r="C3" t="n">
-        <v>28.28017903452562</v>
+        <v>29.25433921813965</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.8698209654743749</v>
+        <v>0.1043392181396428</v>
       </c>
       <c r="E3" t="n">
-        <v>0.7565885119787737</v>
+        <v>0.01088667244199196</v>
       </c>
     </row>
     <row r="4">
@@ -499,16 +499,16 @@
         <v>47</v>
       </c>
       <c r="B4" t="n">
-        <v>29.35</v>
+        <v>29.34999999999999</v>
       </c>
       <c r="C4" t="n">
-        <v>28.88646415724472</v>
+        <v>29.70592308044434</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.4635358427552845</v>
+        <v>0.3559230804443416</v>
       </c>
       <c r="E4" t="n">
-        <v>0.2148654775188518</v>
+        <v>0.1266812391929893</v>
       </c>
     </row>
     <row r="5">
@@ -519,13 +519,13 @@
         <v>29.37</v>
       </c>
       <c r="C5" t="n">
-        <v>28.79124348772752</v>
+        <v>29.52533531188965</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.5787565122724807</v>
+        <v>0.1553353118896439</v>
       </c>
       <c r="E5" t="n">
-        <v>0.3349591004978061</v>
+        <v>0.02412905911985294</v>
       </c>
     </row>
     <row r="6">
@@ -533,16 +533,16 @@
         <v>45</v>
       </c>
       <c r="B6" t="n">
-        <v>29.54</v>
+        <v>29.53999999999999</v>
       </c>
       <c r="C6" t="n">
-        <v>28.69696473790746</v>
+        <v>28.87110710144043</v>
       </c>
       <c r="D6" t="n">
-        <v>-0.8430352620925348</v>
+        <v>-0.6688928985595624</v>
       </c>
       <c r="E6" t="n">
-        <v>0.7107084531314288</v>
+        <v>0.447417709743413</v>
       </c>
     </row>
     <row r="7">
@@ -553,13 +553,13 @@
         <v>29.55</v>
       </c>
       <c r="C7" t="n">
-        <v>29.86126388352603</v>
+        <v>29.35497856140137</v>
       </c>
       <c r="D7" t="n">
-        <v>0.3112638835260277</v>
+        <v>-0.19502143859863</v>
       </c>
       <c r="E7" t="n">
-        <v>0.09688520518770456</v>
+        <v>0.0380333615130792</v>
       </c>
     </row>
     <row r="8">
@@ -570,13 +570,13 @@
         <v>29.75</v>
       </c>
       <c r="C8" t="n">
-        <v>29.59043104121293</v>
+        <v>29.55397605895996</v>
       </c>
       <c r="D8" t="n">
-        <v>-0.1595689587870659</v>
+        <v>-0.1960239410400391</v>
       </c>
       <c r="E8" t="n">
-        <v>0.02546225260838833</v>
+        <v>0.03842538546086871</v>
       </c>
     </row>
     <row r="9">
@@ -587,13 +587,13 @@
         <v>29.84</v>
       </c>
       <c r="C9" t="n">
-        <v>30.47360527894018</v>
+        <v>30.04802513122559</v>
       </c>
       <c r="D9" t="n">
-        <v>0.6336052789401769</v>
+        <v>0.2080251312255825</v>
       </c>
       <c r="E9" t="n">
-        <v>0.4014556495008594</v>
+        <v>0.04327445522142083</v>
       </c>
     </row>
     <row r="10">
@@ -604,13 +604,13 @@
         <v>29.81</v>
       </c>
       <c r="C10" t="n">
-        <v>30.35429894197885</v>
+        <v>29.96916007995605</v>
       </c>
       <c r="D10" t="n">
-        <v>0.5442989419788482</v>
+        <v>0.1591600799560524</v>
       </c>
       <c r="E10" t="n">
-        <v>0.2962613382392936</v>
+        <v>0.025331931051617</v>
       </c>
     </row>
     <row r="11">
@@ -621,13 +621,13 @@
         <v>29.92</v>
       </c>
       <c r="C11" t="n">
-        <v>30.19960459309228</v>
+        <v>29.92043113708496</v>
       </c>
       <c r="D11" t="n">
-        <v>0.2796045930922801</v>
+        <v>0.0004311370849592322</v>
       </c>
       <c r="E11" t="n">
-        <v>0.07817872847829956</v>
+        <v>1.858791860271442e-07</v>
       </c>
     </row>
     <row r="12">
@@ -638,13 +638,13 @@
         <v>29.98</v>
       </c>
       <c r="C12" t="n">
-        <v>29.54863326317109</v>
+        <v>29.84786033630371</v>
       </c>
       <c r="D12" t="n">
-        <v>-0.4313667368289096</v>
+        <v>-0.132139663696293</v>
       </c>
       <c r="E12" t="n">
-        <v>0.1860772616424217</v>
+        <v>0.01746089072176943</v>
       </c>
     </row>
     <row r="13">
@@ -652,16 +652,16 @@
         <v>38</v>
       </c>
       <c r="B13" t="n">
-        <v>30.04</v>
+        <v>30.03999999999999</v>
       </c>
       <c r="C13" t="n">
-        <v>29.85653219908905</v>
+        <v>30.05769920349121</v>
       </c>
       <c r="D13" t="n">
-        <v>-0.1834678009109503</v>
+        <v>0.0176992034912189</v>
       </c>
       <c r="E13" t="n">
-        <v>0.03366043397110009</v>
+        <v>0.0003132618042235752</v>
       </c>
     </row>
     <row r="14">
@@ -669,16 +669,16 @@
         <v>37</v>
       </c>
       <c r="B14" t="n">
-        <v>30.21</v>
+        <v>30.21000000000001</v>
       </c>
       <c r="C14" t="n">
-        <v>29.40461724422588</v>
+        <v>30.05219078063965</v>
       </c>
       <c r="D14" t="n">
-        <v>-0.8053827557741222</v>
+        <v>-0.1578092193603595</v>
       </c>
       <c r="E14" t="n">
-        <v>0.6486413832983194</v>
+        <v>0.02490374971512607</v>
       </c>
     </row>
     <row r="15">
@@ -689,13 +689,13 @@
         <v>30.22</v>
       </c>
       <c r="C15" t="n">
-        <v>29.82918319365324</v>
+        <v>30.22921562194824</v>
       </c>
       <c r="D15" t="n">
-        <v>-0.3908168063467627</v>
+        <v>0.009215621948243324</v>
       </c>
       <c r="E15" t="n">
-        <v>0.1527377761230831</v>
+        <v>8.492768789294409e-05</v>
       </c>
     </row>
     <row r="16">
@@ -706,13 +706,13 @@
         <v>30.38</v>
       </c>
       <c r="C16" t="n">
-        <v>29.64636299647648</v>
+        <v>30.29749870300293</v>
       </c>
       <c r="D16" t="n">
-        <v>-0.7336370035235191</v>
+        <v>-0.08250129699706577</v>
       </c>
       <c r="E16" t="n">
-        <v>0.538223252938968</v>
+        <v>0.006806464006198052</v>
       </c>
     </row>
     <row r="17">
@@ -723,13 +723,13 @@
         <v>30.44</v>
       </c>
       <c r="C17" t="n">
-        <v>30.33773402865503</v>
+        <v>30.6120433807373</v>
       </c>
       <c r="D17" t="n">
-        <v>-0.1022659713449734</v>
+        <v>0.172043380737307</v>
       </c>
       <c r="E17" t="n">
-        <v>0.01045832889513092</v>
+        <v>0.02959892485552196</v>
       </c>
     </row>
     <row r="18">
@@ -740,13 +740,13 @@
         <v>30.48</v>
       </c>
       <c r="C18" t="n">
-        <v>30.36049336566984</v>
+        <v>30.40457725524902</v>
       </c>
       <c r="D18" t="n">
-        <v>-0.1195066343301612</v>
+        <v>-0.07542274475098054</v>
       </c>
       <c r="E18" t="n">
-        <v>0.01428183564892286</v>
+        <v>0.005688590425771562</v>
       </c>
     </row>
     <row r="19">
@@ -757,13 +757,13 @@
         <v>30.69</v>
       </c>
       <c r="C19" t="n">
-        <v>30.65505704903011</v>
+        <v>30.41995811462402</v>
       </c>
       <c r="D19" t="n">
-        <v>-0.03494295096988864</v>
+        <v>-0.2700418853759743</v>
       </c>
       <c r="E19" t="n">
-        <v>0.001221009822484041</v>
+        <v>0.07292261985741083</v>
       </c>
     </row>
     <row r="20">
@@ -774,13 +774,13 @@
         <v>30.75</v>
       </c>
       <c r="C20" t="n">
-        <v>30.32258370656307</v>
+        <v>30.54005241394043</v>
       </c>
       <c r="D20" t="n">
-        <v>-0.4274162934369308</v>
+        <v>-0.2099475860595703</v>
       </c>
       <c r="E20" t="n">
-        <v>0.1826846878953645</v>
+        <v>0.04407798889224068</v>
       </c>
     </row>
     <row r="21">
@@ -791,13 +791,13 @@
         <v>30.94</v>
       </c>
       <c r="C21" t="n">
-        <v>30.73581033191036</v>
+        <v>30.62829399108887</v>
       </c>
       <c r="D21" t="n">
-        <v>-0.2041896680896436</v>
+        <v>-0.3117060089111305</v>
       </c>
       <c r="E21" t="n">
-        <v>0.0416934205545588</v>
+        <v>0.0971606359913058</v>
       </c>
     </row>
     <row r="22">
@@ -808,13 +808,13 @@
         <v>30.95</v>
       </c>
       <c r="C22" t="n">
-        <v>31.06682419096773</v>
+        <v>30.73287773132324</v>
       </c>
       <c r="D22" t="n">
-        <v>0.1168241909677299</v>
+        <v>-0.2171222686767607</v>
       </c>
       <c r="E22" t="n">
-        <v>0.01364789159526462</v>
+        <v>0.04714207955534344</v>
       </c>
     </row>
     <row r="23">
@@ -825,13 +825,13 @@
         <v>31.02</v>
       </c>
       <c r="C23" t="n">
-        <v>31.71203661379989</v>
+        <v>31.12346458435059</v>
       </c>
       <c r="D23" t="n">
-        <v>0.692036613799889</v>
+        <v>0.1034645843505899</v>
       </c>
       <c r="E23" t="n">
-        <v>0.4789146748396167</v>
+        <v>0.01070492021484034</v>
       </c>
     </row>
     <row r="24">
@@ -842,13 +842,13 @@
         <v>31.12</v>
       </c>
       <c r="C24" t="n">
-        <v>32.12226057527928</v>
+        <v>31.30785179138184</v>
       </c>
       <c r="D24" t="n">
-        <v>1.002260575279283</v>
+        <v>0.1878517913818314</v>
       </c>
       <c r="E24" t="n">
-        <v>1.00452626075916</v>
+        <v>0.0352882955253631</v>
       </c>
     </row>
     <row r="25">
@@ -859,13 +859,13 @@
         <v>31.28</v>
       </c>
       <c r="C25" t="n">
-        <v>32.26900250503424</v>
+        <v>31.35338401794434</v>
       </c>
       <c r="D25" t="n">
-        <v>0.989002505034243</v>
+        <v>0.0733840179443348</v>
       </c>
       <c r="E25" t="n">
-        <v>0.9781259549640079</v>
+        <v>0.005385214089654452</v>
       </c>
     </row>
     <row r="26">
@@ -876,13 +876,13 @@
         <v>31.38</v>
       </c>
       <c r="C26" t="n">
-        <v>32.11758947928325</v>
+        <v>31.22195243835449</v>
       </c>
       <c r="D26" t="n">
-        <v>0.7375894792832476</v>
+        <v>-0.1580475616455033</v>
       </c>
       <c r="E26" t="n">
-        <v>0.5440382399493323</v>
+        <v>0.02497903174208916</v>
       </c>
     </row>
     <row r="27">
@@ -893,13 +893,13 @@
         <v>31.58</v>
       </c>
       <c r="C27" t="n">
-        <v>32.53827326168924</v>
+        <v>31.44917106628418</v>
       </c>
       <c r="D27" t="n">
-        <v>0.9582732616892429</v>
+        <v>-0.1308289337158186</v>
       </c>
       <c r="E27" t="n">
-        <v>0.9182876440685401</v>
+        <v>0.01711620989721806</v>
       </c>
     </row>
     <row r="28">
@@ -907,16 +907,16 @@
         <v>23</v>
       </c>
       <c r="B28" t="n">
-        <v>31.65</v>
+        <v>31.65000000000001</v>
       </c>
       <c r="C28" t="n">
-        <v>32.52980955291806</v>
+        <v>31.89203453063965</v>
       </c>
       <c r="D28" t="n">
-        <v>0.8798095529180614</v>
+        <v>0.2420345306396428</v>
       </c>
       <c r="E28" t="n">
-        <v>0.7740648494058791</v>
+        <v>0.05858071402195217</v>
       </c>
     </row>
     <row r="29">
@@ -927,13 +927,13 @@
         <v>31.88</v>
       </c>
       <c r="C29" t="n">
-        <v>33.277970159239</v>
+        <v>32.54359817504883</v>
       </c>
       <c r="D29" t="n">
-        <v>1.397970159238998</v>
+        <v>0.6635981750488327</v>
       </c>
       <c r="E29" t="n">
-        <v>1.954320566122709</v>
+        <v>0.4403625379281412</v>
       </c>
     </row>
     <row r="30">
@@ -944,13 +944,13 @@
         <v>32.28</v>
       </c>
       <c r="C30" t="n">
-        <v>32.85379537904976</v>
+        <v>32.46515274047852</v>
       </c>
       <c r="D30" t="n">
-        <v>0.5737953790497556</v>
+        <v>0.1851527404785145</v>
       </c>
       <c r="E30" t="n">
-        <v>0.3292411370188528</v>
+        <v>0.03428153730670414</v>
       </c>
     </row>
     <row r="31">
@@ -961,13 +961,13 @@
         <v>32.45</v>
       </c>
       <c r="C31" t="n">
-        <v>32.96916922584683</v>
+        <v>32.5944709777832</v>
       </c>
       <c r="D31" t="n">
-        <v>0.5191692258468237</v>
+        <v>0.1444709777832003</v>
       </c>
       <c r="E31" t="n">
-        <v>0.2695366850663902</v>
+        <v>0.02087186342163395</v>
       </c>
     </row>
     <row r="32">
@@ -975,16 +975,16 @@
         <v>19</v>
       </c>
       <c r="B32" t="n">
-        <v>32.85</v>
+        <v>32.84999999999999</v>
       </c>
       <c r="C32" t="n">
-        <v>33.13367271978353</v>
+        <v>32.88671493530273</v>
       </c>
       <c r="D32" t="n">
-        <v>0.2836727197835245</v>
+        <v>0.03671493530274006</v>
       </c>
       <c r="E32" t="n">
-        <v>0.080470211949382</v>
+        <v>0.001347986474284388</v>
       </c>
     </row>
     <row r="33">
@@ -992,16 +992,16 @@
         <v>18</v>
       </c>
       <c r="B33" t="n">
-        <v>32.9</v>
+        <v>32.90000000000001</v>
       </c>
       <c r="C33" t="n">
-        <v>33.22534331497836</v>
+        <v>33.03625106811523</v>
       </c>
       <c r="D33" t="n">
-        <v>0.3253433149783618</v>
+        <v>0.1362510681152287</v>
       </c>
       <c r="E33" t="n">
-        <v>0.1058482726011095</v>
+        <v>0.01856435356254069</v>
       </c>
     </row>
     <row r="34">
@@ -1009,16 +1009,16 @@
         <v>17</v>
       </c>
       <c r="B34" t="n">
-        <v>33.1</v>
+        <v>33.09999999999999</v>
       </c>
       <c r="C34" t="n">
-        <v>33.21840007594129</v>
+        <v>32.95847702026367</v>
       </c>
       <c r="D34" t="n">
-        <v>0.1184000759412882</v>
+        <v>-0.1415229797363224</v>
       </c>
       <c r="E34" t="n">
-        <v>0.01401857798290281</v>
+        <v>0.02002875379344753</v>
       </c>
     </row>
     <row r="35">
@@ -1026,16 +1026,16 @@
         <v>16</v>
       </c>
       <c r="B35" t="n">
-        <v>33.4</v>
+        <v>33.40000000000001</v>
       </c>
       <c r="C35" t="n">
-        <v>34.21330507641433</v>
+        <v>33.7332878112793</v>
       </c>
       <c r="D35" t="n">
-        <v>0.8133050764143306</v>
+        <v>0.3332878112792912</v>
       </c>
       <c r="E35" t="n">
-        <v>0.6614651473213201</v>
+        <v>0.1110807651473404</v>
       </c>
     </row>
     <row r="36">
@@ -1046,13 +1046,13 @@
         <v>33.7</v>
       </c>
       <c r="C36" t="n">
-        <v>33.99777500965789</v>
+        <v>33.6826286315918</v>
       </c>
       <c r="D36" t="n">
-        <v>0.2977750096578902</v>
+        <v>-0.01737136840820597</v>
       </c>
       <c r="E36" t="n">
-        <v>0.08866995637675658</v>
+        <v>0.0003017644403736163</v>
       </c>
     </row>
     <row r="37">
@@ -1060,16 +1060,16 @@
         <v>14</v>
       </c>
       <c r="B37" t="n">
-        <v>34.1</v>
+        <v>34.09999999999999</v>
       </c>
       <c r="C37" t="n">
-        <v>34.04644958257992</v>
+        <v>33.8400993347168</v>
       </c>
       <c r="D37" t="n">
-        <v>-0.05355041742008382</v>
+        <v>-0.2599006652831974</v>
       </c>
       <c r="E37" t="n">
-        <v>0.002867647205865216</v>
+        <v>0.06754835581464863</v>
       </c>
     </row>
     <row r="38">
@@ -1077,16 +1077,16 @@
         <v>13</v>
       </c>
       <c r="B38" t="n">
-        <v>34.4</v>
+        <v>34.40000000000001</v>
       </c>
       <c r="C38" t="n">
-        <v>34.57601968097843</v>
+        <v>34.36728286743164</v>
       </c>
       <c r="D38" t="n">
-        <v>0.1760196809784276</v>
+        <v>-0.03271713256836506</v>
       </c>
       <c r="E38" t="n">
-        <v>0.03098292809174742</v>
+        <v>0.001070410763495974</v>
       </c>
     </row>
     <row r="39">
@@ -1094,16 +1094,16 @@
         <v>12</v>
       </c>
       <c r="B39" t="n">
-        <v>34.9</v>
+        <v>34.90000000000001</v>
       </c>
       <c r="C39" t="n">
-        <v>34.85083618170182</v>
+        <v>34.92761611938477</v>
       </c>
       <c r="D39" t="n">
-        <v>-0.04916381829818306</v>
+        <v>0.02761611938475994</v>
       </c>
       <c r="E39" t="n">
-        <v>0.002417081029656759</v>
+        <v>0.0007626500498733137</v>
       </c>
     </row>
     <row r="40">
@@ -1114,13 +1114,13 @@
         <v>35.3</v>
       </c>
       <c r="C40" t="n">
-        <v>35.9687543924692</v>
+        <v>35.70381546020508</v>
       </c>
       <c r="D40" t="n">
-        <v>0.6687543924692037</v>
+        <v>0.403815460205081</v>
       </c>
       <c r="E40" t="n">
-        <v>0.4472324374468536</v>
+        <v>0.1630669259006413</v>
       </c>
     </row>
     <row r="41">
@@ -1131,13 +1131,13 @@
         <v>35.7</v>
       </c>
       <c r="C41" t="n">
-        <v>36.10000759518975</v>
+        <v>35.95959854125977</v>
       </c>
       <c r="D41" t="n">
-        <v>0.4000075951897486</v>
+        <v>0.2595985412597628</v>
       </c>
       <c r="E41" t="n">
-        <v>0.1600060762094858</v>
+        <v>0.06739140262419677</v>
       </c>
     </row>
     <row r="42">
@@ -1148,13 +1148,13 @@
         <v>36.3</v>
       </c>
       <c r="C42" t="n">
-        <v>35.91907778380174</v>
+        <v>36.04191970825195</v>
       </c>
       <c r="D42" t="n">
-        <v>-0.3809222161982575</v>
+        <v>-0.258080291748044</v>
       </c>
       <c r="E42" t="n">
-        <v>0.145101734793392</v>
+        <v>0.06660543698875553</v>
       </c>
     </row>
     <row r="43">
@@ -1165,13 +1165,13 @@
         <v>36.8</v>
       </c>
       <c r="C43" t="n">
-        <v>36.40238053655096</v>
+        <v>36.59153366088867</v>
       </c>
       <c r="D43" t="n">
-        <v>-0.3976194634490327</v>
+        <v>-0.2084663391113253</v>
       </c>
       <c r="E43" t="n">
-        <v>0.1581012377134966</v>
+        <v>0.04345821454247807</v>
       </c>
     </row>
     <row r="44">
@@ -1182,13 +1182,13 @@
         <v>37.3</v>
       </c>
       <c r="C44" t="n">
-        <v>36.34026366487587</v>
+        <v>37.04032516479492</v>
       </c>
       <c r="D44" t="n">
-        <v>-0.959736335124127</v>
+        <v>-0.2596748352050753</v>
       </c>
       <c r="E44" t="n">
-        <v>0.9210938329574907</v>
+        <v>0.067431020038783</v>
       </c>
     </row>
     <row r="45">
@@ -1196,16 +1196,16 @@
         <v>6</v>
       </c>
       <c r="B45" t="n">
-        <v>37.9</v>
+        <v>37.90000000000001</v>
       </c>
       <c r="C45" t="n">
-        <v>37.45542092048556</v>
+        <v>37.8508186340332</v>
       </c>
       <c r="D45" t="n">
-        <v>-0.4445790795144404</v>
+        <v>-0.04918136596680256</v>
       </c>
       <c r="E45" t="n">
-        <v>0.1976505579419071</v>
+        <v>0.002418806758360565</v>
       </c>
     </row>
     <row r="46">
@@ -1216,13 +1216,13 @@
         <v>38.5</v>
       </c>
       <c r="C46" t="n">
-        <v>38.17963449233827</v>
+        <v>38.36010360717773</v>
       </c>
       <c r="D46" t="n">
-        <v>-0.3203655076617338</v>
+        <v>-0.1398963928222656</v>
       </c>
       <c r="E46" t="n">
-        <v>0.1026340584993604</v>
+        <v>0.01957100072468165</v>
       </c>
     </row>
     <row r="47">
@@ -1230,16 +1230,16 @@
         <v>4</v>
       </c>
       <c r="B47" t="n">
-        <v>38.9</v>
+        <v>38.90000000000001</v>
       </c>
       <c r="C47" t="n">
-        <v>38.58431861107851</v>
+        <v>38.94926071166992</v>
       </c>
       <c r="D47" t="n">
-        <v>-0.3156813889214902</v>
+        <v>0.04926071166991619</v>
       </c>
       <c r="E47" t="n">
-        <v>0.09965473931140117</v>
+        <v>0.002426617714226617</v>
       </c>
     </row>
     <row r="48">
@@ -1247,16 +1247,16 @@
         <v>3</v>
       </c>
       <c r="B48" t="n">
-        <v>39.4</v>
+        <v>39.40000000000001</v>
       </c>
       <c r="C48" t="n">
-        <v>38.90683823342697</v>
+        <v>39.48398208618164</v>
       </c>
       <c r="D48" t="n">
-        <v>-0.4931617665730244</v>
+        <v>0.08398208618163494</v>
       </c>
       <c r="E48" t="n">
-        <v>0.2432085280094262</v>
+        <v>0.007052990799419559</v>
       </c>
     </row>
     <row r="49">
@@ -1264,16 +1264,16 @@
         <v>2</v>
       </c>
       <c r="B49" t="n">
-        <v>39.9</v>
+        <v>39.90000000000001</v>
       </c>
       <c r="C49" t="n">
-        <v>39.41233102678765</v>
+        <v>39.5393180847168</v>
       </c>
       <c r="D49" t="n">
-        <v>-0.4876689732123509</v>
+        <v>-0.3606819152832088</v>
       </c>
       <c r="E49" t="n">
-        <v>0.2378210274339886</v>
+        <v>0.1300914440123638</v>
       </c>
     </row>
     <row r="50">
@@ -1281,16 +1281,16 @@
         <v>1</v>
       </c>
       <c r="B50" t="n">
-        <v>40.1</v>
+        <v>40.09999999999999</v>
       </c>
       <c r="C50" t="n">
-        <v>39.24870500583931</v>
+        <v>40.14670181274414</v>
       </c>
       <c r="D50" t="n">
-        <v>-0.8512949941606962</v>
+        <v>0.04670181274414631</v>
       </c>
       <c r="E50" t="n">
-        <v>0.7247031670830598</v>
+        <v>0.002181059313589307</v>
       </c>
     </row>
     <row r="51">
@@ -1298,16 +1298,16 @@
         <v>0</v>
       </c>
       <c r="B51" t="n">
-        <v>40.6</v>
+        <v>40.59999999999999</v>
       </c>
       <c r="C51" t="n">
-        <v>39.33456577636483</v>
+        <v>40.69865036010742</v>
       </c>
       <c r="D51" t="n">
-        <v>-1.265434223635175</v>
+        <v>0.09865036010742756</v>
       </c>
       <c r="E51" t="n">
-        <v>1.601323774347159</v>
+        <v>0.009731893549325134</v>
       </c>
     </row>
     <row r="52">
@@ -1318,11 +1318,11 @@
       </c>
       <c r="B52" t="inlineStr"/>
       <c r="C52" t="n">
-        <v>-0.008685308628653132</v>
+        <v>0.04815361022947684</v>
       </c>
       <c r="D52" t="inlineStr"/>
       <c r="E52" t="n">
-        <v>18.1450358373095</v>
+        <v>2.654464649066489</v>
       </c>
     </row>
     <row r="53">
@@ -1335,7 +1335,7 @@
       <c r="C53" t="inlineStr"/>
       <c r="D53" t="inlineStr"/>
       <c r="E53" t="n">
-        <v>0.36290071674619</v>
+        <v>0.05308929298132978</v>
       </c>
     </row>
   </sheetData>

</xml_diff>